<commit_message>
Update Diagramme de Gantt de suivi de date1.xlsx
</commit_message>
<xml_diff>
--- a/Jalon 1/Diagramme de Gantt de suivi de date1.xlsx
+++ b/Jalon 1/Diagramme de Gantt de suivi de date1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E10688-CBBB-4C5B-82D5-09E8396F8DFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91047C27-1C44-4406-8585-F59E7BAB4557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vert" sheetId="18" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="54">
   <si>
     <t>Date de début du projet :</t>
   </si>
@@ -197,6 +197,9 @@
   </si>
   <si>
     <t xml:space="preserve">PROJET AP </t>
+  </si>
+  <si>
+    <t>(modification à faire)</t>
   </si>
 </sst>
 </file>
@@ -1288,6 +1291,13 @@
   </cellStyles>
   <dxfs count="18">
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color theme="8" tint="-0.499984740745262"/>
       </font>
@@ -1327,13 +1337,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <border>
@@ -1660,7 +1663,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8EE7DA96-2148-4820-AB9C-230AD0CA6702}" name="Jalons34" displayName="Jalons34" ref="B8:F45" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8EE7DA96-2148-4820-AB9C-230AD0CA6702}" name="Jalons34" displayName="Jalons34" ref="B8:F45" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="B8:F45" xr:uid="{29E5A880-80D5-4B65-B5FB-8FB3913D3D27}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1952,8 +1955,8 @@
   </sheetPr>
   <dimension ref="A1:BK48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A17" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="30" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
@@ -6198,7 +6201,9 @@
     </row>
     <row r="31" spans="1:63" s="1" customFormat="1" ht="30" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6"/>
-      <c r="B31" s="45"/>
+      <c r="B31" s="45" t="s">
+        <v>53</v>
+      </c>
       <c r="C31" s="11"/>
       <c r="D31" s="39"/>
       <c r="E31" s="38"/>
@@ -8781,17 +8786,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10:BK10 H20:BK45 I11:BK11 I13:BK14 I12:N12 P12:BK12 H15:N19 P15:BK19">
-    <cfRule type="expression" dxfId="2" priority="6">
+    <cfRule type="expression" dxfId="3" priority="6">
       <formula>H$7&lt;=Aujourd’hui</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:BK10 H20:BK45 I11:BK11 I13:BK14 I12:N12 P12:BK12 H15:N19 P15:BK19">
-    <cfRule type="expression" dxfId="1" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="5" stopIfTrue="1">
       <formula>AND(H$7&gt;=$E9+1,H$7&lt;=$E9+$F9-2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:BK8">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>H$7&lt;=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8910,25 +8915,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="22a266b9fa9a230c5a512669d8b298c3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="eddc33fff6b14141ee5c74a0d29ea6a1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -9204,6 +9190,25 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -9214,18 +9219,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D0BFDC8-3FC5-4B1A-A529-197CCE587781}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51416DF5-5CF4-40FC-9B7A-D5A4568A710D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9246,6 +9239,18 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D0BFDC8-3FC5-4B1A-A529-197CCE587781}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69D04340-DBA0-4EBA-8015-0619D6CE3F7C}">
   <ds:schemaRefs>

</xml_diff>